<commit_message>
modification in test scripts
</commit_message>
<xml_diff>
--- a/Excel/testdata.xlsx
+++ b/Excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_Selenium\AppiumMobileAutomationFramework\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58295AEC-B2B5-4F75-B3A6-3730B8D9D8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C4E054-83CB-46B9-BE0B-21CCB70A9DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddToCartData" sheetId="3" r:id="rId1"/>
@@ -437,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC812C77-110A-4C8A-8FAA-129257CB6E93}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1353D2-FB83-4FCF-9B78-E9E7A0A6934F}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>